<commit_message>
Fixed Excel Building Data Upload
</commit_message>
<xml_diff>
--- a/Notes/Data.xlsx
+++ b/Notes/Data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Buildings" sheetId="3" r:id="rId1"/>
-    <sheet name="Units" sheetId="2" r:id="rId2"/>
-    <sheet name="WorldCountries" sheetId="1" r:id="rId3"/>
-    <sheet name="CountryUnitArmyCode" sheetId="4" r:id="rId4"/>
+    <sheet name="BuildingType" sheetId="5" r:id="rId2"/>
+    <sheet name="Units" sheetId="2" r:id="rId3"/>
+    <sheet name="WorldCountries" sheetId="1" r:id="rId4"/>
+    <sheet name="CountryUnitArmyCode" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="132">
   <si>
     <t>US</t>
   </si>
@@ -402,6 +403,27 @@
   </si>
   <si>
     <t>baseFoodGrowth</t>
+  </si>
+  <si>
+    <t>buildingTypeCode</t>
+  </si>
+  <si>
+    <t>buildingTypeName</t>
+  </si>
+  <si>
+    <t>Economic</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Military</t>
   </si>
 </sst>
 </file>
@@ -457,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -465,7 +487,10 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,23 +774,23 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -773,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>62</v>
@@ -793,16 +818,16 @@
       <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>65</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="9" t="s">
         <v>67</v>
       </c>
       <c r="M1" s="7" t="s">
@@ -819,37 +844,37 @@
       <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
         <v>1000</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="8">
         <v>1000</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="8">
         <v>1000</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="6">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6">
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1</v>
+      </c>
+      <c r="N2" s="8">
         <v>1</v>
       </c>
     </row>
@@ -860,37 +885,37 @@
       <c r="B3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
         <v>100</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <v>50000</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="8">
         <v>50000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="8">
         <v>50000</v>
       </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
         <v>2</v>
       </c>
       <c r="K3" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="10">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6">
+      <c r="M3" s="8">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
         <v>50</v>
       </c>
     </row>
@@ -901,37 +926,37 @@
       <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
         <v>2000</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
         <v>1000000</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="8">
         <v>1000000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="8">
         <v>1000000</v>
       </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
         <v>3</v>
       </c>
       <c r="K4" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="10">
         <v>1.000006</v>
       </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6">
+      <c r="M4" s="8">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8">
         <v>1000</v>
       </c>
     </row>
@@ -942,37 +967,37 @@
       <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
         <v>100000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="8">
         <v>100000000</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="8">
         <v>100000000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="8">
         <v>100000000</v>
       </c>
-      <c r="I5" s="6">
-        <v>1</v>
-      </c>
-      <c r="J5" s="6">
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
         <v>4</v>
       </c>
       <c r="K5" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="6">
-        <v>1</v>
-      </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
         <v>200000</v>
       </c>
     </row>
@@ -983,37 +1008,37 @@
       <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
         <v>200000</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="8">
         <v>500000000</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="8">
         <v>500000000</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="8">
         <v>500000000</v>
       </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
         <v>5</v>
       </c>
       <c r="K6" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="10">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M6" s="6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8">
         <v>1000000</v>
       </c>
     </row>
@@ -1024,37 +1049,37 @@
       <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
         <v>1000000</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="8">
         <v>10000000000</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="8">
         <v>10000000000</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="8">
         <v>10000000000</v>
       </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
         <v>6</v>
       </c>
       <c r="K7" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
         <v>10000</v>
       </c>
     </row>
@@ -1065,8 +1090,38 @@
       <c r="B8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="6">
-        <v>0</v>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1076,8 +1131,38 @@
       <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="6">
-        <v>0</v>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>100</v>
+      </c>
+      <c r="F9" s="8">
+        <v>50000</v>
+      </c>
+      <c r="G9" s="8">
+        <v>50000</v>
+      </c>
+      <c r="H9" s="8">
+        <v>50000</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1087,8 +1172,38 @@
       <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6">
-        <v>0</v>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1.000006</v>
+      </c>
+      <c r="M10" s="8">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1098,8 +1213,38 @@
       <c r="B11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="6">
-        <v>0</v>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>100000</v>
+      </c>
+      <c r="F11" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="G11" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="H11" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="10">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8">
+        <v>200000</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1109,8 +1254,38 @@
       <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="6">
-        <v>0</v>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>200000</v>
+      </c>
+      <c r="F12" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="G12" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="H12" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="10">
+        <v>1.0035000000000001</v>
+      </c>
+      <c r="M12" s="8">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8">
+        <v>1000000</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1120,8 +1295,38 @@
       <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="6">
-        <v>0</v>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="F13" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="G13" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="H13" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M13" s="8">
+        <v>1</v>
+      </c>
+      <c r="N13" s="8">
+        <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1131,37 +1336,37 @@
       <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="8">
         <v>8</v>
       </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
         <v>1000</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="8">
         <v>1000</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="8">
         <v>1000</v>
       </c>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
-      <c r="J14" s="6">
+      <c r="I14" s="8">
+        <v>1</v>
+      </c>
+      <c r="J14" s="8">
         <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>111</v>
       </c>
-      <c r="L14" s="6">
-        <v>1</v>
-      </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6">
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1172,37 +1377,37 @@
       <c r="B15" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
         <v>200</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="8">
         <v>100000</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="8">
         <v>100000</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="8">
         <v>100000</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6">
+      <c r="I15" s="8">
+        <v>1</v>
+      </c>
+      <c r="J15" s="8">
         <v>2</v>
       </c>
       <c r="K15" t="s">
         <v>111</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="10">
         <v>150</v>
       </c>
-      <c r="M15" s="6">
-        <v>1</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="M15" s="8">
+        <v>1</v>
+      </c>
+      <c r="N15" s="8">
         <v>8</v>
       </c>
     </row>
@@ -1213,37 +1418,37 @@
       <c r="B16" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
         <v>2000</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="8">
         <v>1000000</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="8">
         <v>1000000</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="8">
         <v>1000000</v>
       </c>
-      <c r="I16" s="6">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6">
+      <c r="I16" s="8">
+        <v>1</v>
+      </c>
+      <c r="J16" s="8">
         <v>3</v>
       </c>
       <c r="K16" t="s">
         <v>111</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="10">
         <v>2000</v>
       </c>
-      <c r="M16" s="6">
-        <v>1</v>
-      </c>
-      <c r="N16" s="6">
+      <c r="M16" s="8">
+        <v>1</v>
+      </c>
+      <c r="N16" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1254,37 +1459,37 @@
       <c r="B17" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
         <v>100000</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="8">
         <v>100000000</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="8">
         <v>100000000</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="8">
         <v>100000000</v>
       </c>
-      <c r="I17" s="6">
-        <v>1</v>
-      </c>
-      <c r="J17" s="6">
+      <c r="I17" s="8">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8">
         <v>4</v>
       </c>
       <c r="K17" t="s">
         <v>111</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="10">
         <v>250000</v>
       </c>
-      <c r="M17" s="6">
-        <v>1</v>
-      </c>
-      <c r="N17" s="6">
+      <c r="M17" s="8">
+        <v>1</v>
+      </c>
+      <c r="N17" s="8">
         <v>10000</v>
       </c>
     </row>
@@ -1295,37 +1500,37 @@
       <c r="B18" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
         <v>200000</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="8">
         <v>500000000</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="8">
         <v>500000000</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="8">
         <v>500000000</v>
       </c>
-      <c r="I18" s="6">
-        <v>1</v>
-      </c>
-      <c r="J18" s="6">
+      <c r="I18" s="8">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8">
         <v>5</v>
       </c>
       <c r="K18" t="s">
         <v>111</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="10">
         <v>1500000</v>
       </c>
-      <c r="M18" s="6">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18" s="8">
+        <v>1</v>
+      </c>
+      <c r="N18" s="8">
         <v>50000</v>
       </c>
     </row>
@@ -1336,37 +1541,37 @@
       <c r="B19" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
         <v>1000000</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="8">
         <v>10000000000</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="8">
         <v>10000000000</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="8">
         <v>10000000000</v>
       </c>
-      <c r="I19" s="6">
-        <v>1</v>
-      </c>
-      <c r="J19" s="6">
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
         <v>6</v>
       </c>
       <c r="K19" t="s">
         <v>111</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="10">
         <v>40000000</v>
       </c>
-      <c r="M19" s="6">
-        <v>1</v>
-      </c>
-      <c r="N19" s="6">
+      <c r="M19" s="8">
+        <v>1</v>
+      </c>
+      <c r="N19" s="8">
         <v>100000</v>
       </c>
     </row>
@@ -1377,37 +1582,37 @@
       <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="8">
         <v>5</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="8">
         <v>2</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="8">
         <v>2000</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="8">
         <v>2000</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="8">
         <v>2000</v>
       </c>
-      <c r="I20" s="6">
-        <v>1</v>
-      </c>
-      <c r="J20" s="6">
+      <c r="I20" s="8">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8">
         <v>1</v>
       </c>
       <c r="K20" t="s">
         <v>124</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="10">
         <v>10</v>
       </c>
-      <c r="M20" s="6">
-        <v>1</v>
-      </c>
-      <c r="N20" s="6">
+      <c r="M20" s="8">
+        <v>1</v>
+      </c>
+      <c r="N20" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1418,37 +1623,37 @@
       <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
         <v>100</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="8">
         <v>50000</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="8">
         <v>50000</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="8">
         <v>50000</v>
       </c>
-      <c r="I21" s="6">
-        <v>1</v>
-      </c>
-      <c r="J21" s="6">
+      <c r="I21" s="8">
+        <v>1</v>
+      </c>
+      <c r="J21" s="8">
         <v>2</v>
       </c>
       <c r="K21" t="s">
         <v>124</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="10">
         <v>375</v>
       </c>
-      <c r="M21" s="6">
-        <v>1</v>
-      </c>
-      <c r="N21" s="6">
+      <c r="M21" s="8">
+        <v>1</v>
+      </c>
+      <c r="N21" s="8">
         <v>20</v>
       </c>
     </row>
@@ -1459,37 +1664,37 @@
       <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
         <v>2000</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="8">
         <v>1000000</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="8">
         <v>1000000</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="8">
         <v>1000000</v>
       </c>
-      <c r="I22" s="6">
-        <v>1</v>
-      </c>
-      <c r="J22" s="6">
+      <c r="I22" s="8">
+        <v>1</v>
+      </c>
+      <c r="J22" s="8">
         <v>3</v>
       </c>
       <c r="K22" t="s">
         <v>124</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="10">
         <v>10000</v>
       </c>
-      <c r="M22" s="6">
-        <v>1</v>
-      </c>
-      <c r="N22" s="6">
+      <c r="M22" s="8">
+        <v>1</v>
+      </c>
+      <c r="N22" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1500,37 +1705,37 @@
       <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
         <v>10000</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="8">
         <v>10000000</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="8">
         <v>10000000</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="8">
         <v>10000000</v>
       </c>
-      <c r="I23" s="6">
-        <v>1</v>
-      </c>
-      <c r="J23" s="6">
+      <c r="I23" s="8">
+        <v>1</v>
+      </c>
+      <c r="J23" s="8">
         <v>4</v>
       </c>
       <c r="K23" t="s">
         <v>124</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="10">
         <v>125000</v>
       </c>
-      <c r="M23" s="6">
-        <v>1</v>
-      </c>
-      <c r="N23" s="6">
+      <c r="M23" s="8">
+        <v>1</v>
+      </c>
+      <c r="N23" s="8">
         <v>500</v>
       </c>
     </row>
@@ -1541,37 +1746,37 @@
       <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6">
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
         <v>200000</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="8">
         <v>500000000</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="8">
         <v>500000000</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="8">
         <v>500000000</v>
       </c>
-      <c r="I24" s="6">
-        <v>1</v>
-      </c>
-      <c r="J24" s="6">
+      <c r="I24" s="8">
+        <v>1</v>
+      </c>
+      <c r="J24" s="8">
         <v>5</v>
       </c>
       <c r="K24" t="s">
         <v>124</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="10">
         <v>7500000</v>
       </c>
-      <c r="M24" s="6">
-        <v>1</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24" s="8">
+        <v>1</v>
+      </c>
+      <c r="N24" s="8">
         <v>10000</v>
       </c>
     </row>
@@ -1582,37 +1787,37 @@
       <c r="B25" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="6">
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
         <v>1000000</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="8">
         <v>10000000000</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="8">
         <v>10000000000</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="8">
         <v>10000000000</v>
       </c>
-      <c r="I25" s="6">
-        <v>1</v>
-      </c>
-      <c r="J25" s="6">
+      <c r="I25" s="8">
+        <v>1</v>
+      </c>
+      <c r="J25" s="8">
         <v>6</v>
       </c>
       <c r="K25" t="s">
         <v>124</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="10">
         <v>200000000</v>
       </c>
-      <c r="M25" s="6">
-        <v>1</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25" s="8">
+        <v>1</v>
+      </c>
+      <c r="N25" s="8">
         <v>10000</v>
       </c>
     </row>
@@ -1623,8 +1828,38 @@
       <c r="B26" t="s">
         <v>110</v>
       </c>
-      <c r="D26">
-        <v>0</v>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="8">
+        <v>1</v>
+      </c>
+      <c r="J26" s="8">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+      <c r="M26" s="8">
+        <v>1</v>
+      </c>
+      <c r="N26" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1634,8 +1869,38 @@
       <c r="B27" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="6">
-        <v>0</v>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8">
+        <v>100</v>
+      </c>
+      <c r="F27" s="8">
+        <v>50000</v>
+      </c>
+      <c r="G27" s="8">
+        <v>50000</v>
+      </c>
+      <c r="H27" s="8">
+        <v>50000</v>
+      </c>
+      <c r="I27" s="8">
+        <v>1</v>
+      </c>
+      <c r="J27" s="8">
+        <v>2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="10">
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="M27" s="8">
+        <v>1</v>
+      </c>
+      <c r="N27" s="8">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1645,8 +1910,38 @@
       <c r="B28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="6">
-        <v>0</v>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="I28" s="8">
+        <v>1</v>
+      </c>
+      <c r="J28" s="8">
+        <v>3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" s="10">
+        <v>1.000006</v>
+      </c>
+      <c r="M28" s="8">
+        <v>1</v>
+      </c>
+      <c r="N28" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -1656,8 +1951,38 @@
       <c r="B29" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="6">
-        <v>0</v>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>100000</v>
+      </c>
+      <c r="F29" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="G29" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="H29" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="I29" s="8">
+        <v>1</v>
+      </c>
+      <c r="J29" s="8">
+        <v>4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="10">
+        <v>1</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1</v>
+      </c>
+      <c r="N29" s="8">
+        <v>200000</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1667,8 +1992,38 @@
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="6">
-        <v>0</v>
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <v>200000</v>
+      </c>
+      <c r="F30" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="G30" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="H30" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="I30" s="8">
+        <v>1</v>
+      </c>
+      <c r="J30" s="8">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>72</v>
+      </c>
+      <c r="L30" s="10">
+        <v>1.0035000000000001</v>
+      </c>
+      <c r="M30" s="8">
+        <v>1</v>
+      </c>
+      <c r="N30" s="8">
+        <v>1000000</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1678,8 +2033,38 @@
       <c r="B31" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="6">
-        <v>0</v>
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="F31" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="G31" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="H31" s="8">
+        <v>10000000000</v>
+      </c>
+      <c r="I31" s="8">
+        <v>1</v>
+      </c>
+      <c r="J31" s="8">
+        <v>6</v>
+      </c>
+      <c r="K31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M31" s="8">
+        <v>1</v>
+      </c>
+      <c r="N31" s="8">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -1689,6 +2074,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
@@ -2422,7 +2873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -2546,7 +2997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added a new stat to buildings
To handle Multipliers vs adders
</commit_message>
<xml_diff>
--- a/Notes/Data.xlsx
+++ b/Notes/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="28800" windowHeight="12420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Buildings" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
   <si>
     <t>US</t>
   </si>
@@ -424,6 +424,21 @@
   </si>
   <si>
     <t>Military</t>
+  </si>
+  <si>
+    <t>statAdder</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Aircraft Carrier</t>
+  </si>
+  <si>
+    <t>unit018</t>
   </si>
 </sst>
 </file>
@@ -771,29 +786,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -830,14 +846,17 @@
       <c r="L1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -871,14 +890,17 @@
       <c r="L2" s="10">
         <v>1</v>
       </c>
-      <c r="M2" s="8">
-        <v>1</v>
+      <c r="M2" s="10">
+        <v>0</v>
       </c>
       <c r="N2" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -912,14 +934,17 @@
       <c r="L3" s="10">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M3" s="8">
-        <v>1</v>
+      <c r="M3" s="10">
+        <v>0</v>
       </c>
       <c r="N3" s="8">
+        <v>1</v>
+      </c>
+      <c r="O3" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -953,14 +978,17 @@
       <c r="L4" s="10">
         <v>1.000006</v>
       </c>
-      <c r="M4" s="8">
-        <v>1</v>
+      <c r="M4" s="10">
+        <v>0</v>
       </c>
       <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="O4" s="8">
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -994,14 +1022,17 @@
       <c r="L5" s="10">
         <v>1</v>
       </c>
-      <c r="M5" s="8">
-        <v>1</v>
+      <c r="M5" s="10">
+        <v>0</v>
       </c>
       <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
         <v>200000</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1035,14 +1066,17 @@
       <c r="L6" s="10">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M6" s="8">
-        <v>1</v>
+      <c r="M6" s="10">
+        <v>0</v>
       </c>
       <c r="N6" s="8">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8">
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1076,14 +1110,17 @@
       <c r="L7" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M7" s="8">
-        <v>1</v>
+      <c r="M7" s="10">
+        <v>0</v>
       </c>
       <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1117,14 +1154,17 @@
       <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="8">
-        <v>1</v>
+      <c r="M8" s="10">
+        <v>0</v>
       </c>
       <c r="N8" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -1158,14 +1198,17 @@
       <c r="L9" s="10">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M9" s="8">
-        <v>1</v>
+      <c r="M9" s="10">
+        <v>0</v>
       </c>
       <c r="N9" s="8">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1199,14 +1242,17 @@
       <c r="L10" s="10">
         <v>1.000006</v>
       </c>
-      <c r="M10" s="8">
-        <v>1</v>
+      <c r="M10" s="10">
+        <v>0</v>
       </c>
       <c r="N10" s="8">
+        <v>1</v>
+      </c>
+      <c r="O10" s="8">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1240,14 +1286,17 @@
       <c r="L11" s="10">
         <v>1</v>
       </c>
-      <c r="M11" s="8">
-        <v>1</v>
+      <c r="M11" s="10">
+        <v>0</v>
       </c>
       <c r="N11" s="8">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8">
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1281,14 +1330,17 @@
       <c r="L12" s="10">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M12" s="8">
-        <v>1</v>
+      <c r="M12" s="10">
+        <v>0</v>
       </c>
       <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
         <v>1000000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1322,14 +1374,17 @@
       <c r="L13" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M13" s="8">
-        <v>1</v>
+      <c r="M13" s="10">
+        <v>0</v>
       </c>
       <c r="N13" s="8">
+        <v>1</v>
+      </c>
+      <c r="O13" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -1363,14 +1418,17 @@
       <c r="L14" s="10">
         <v>1</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="10">
         <v>1</v>
       </c>
       <c r="N14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -1402,16 +1460,19 @@
         <v>111</v>
       </c>
       <c r="L15" s="10">
+        <v>1</v>
+      </c>
+      <c r="M15" s="10">
         <v>150</v>
       </c>
-      <c r="M15" s="8">
-        <v>1</v>
-      </c>
       <c r="N15" s="8">
+        <v>1</v>
+      </c>
+      <c r="O15" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1443,16 +1504,19 @@
         <v>111</v>
       </c>
       <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="10">
         <v>2000</v>
       </c>
-      <c r="M16" s="8">
-        <v>1</v>
-      </c>
       <c r="N16" s="8">
+        <v>1</v>
+      </c>
+      <c r="O16" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -1484,16 +1548,19 @@
         <v>111</v>
       </c>
       <c r="L17" s="10">
+        <v>1</v>
+      </c>
+      <c r="M17" s="10">
         <v>250000</v>
       </c>
-      <c r="M17" s="8">
-        <v>1</v>
-      </c>
       <c r="N17" s="8">
+        <v>1</v>
+      </c>
+      <c r="O17" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -1525,16 +1592,19 @@
         <v>111</v>
       </c>
       <c r="L18" s="10">
+        <v>1</v>
+      </c>
+      <c r="M18" s="10">
         <v>1500000</v>
       </c>
-      <c r="M18" s="8">
-        <v>1</v>
-      </c>
       <c r="N18" s="8">
+        <v>1</v>
+      </c>
+      <c r="O18" s="8">
         <v>50000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -1566,16 +1636,19 @@
         <v>111</v>
       </c>
       <c r="L19" s="10">
+        <v>1</v>
+      </c>
+      <c r="M19" s="10">
         <v>40000000</v>
       </c>
-      <c r="M19" s="8">
-        <v>1</v>
-      </c>
       <c r="N19" s="8">
+        <v>1</v>
+      </c>
+      <c r="O19" s="8">
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -1607,16 +1680,19 @@
         <v>124</v>
       </c>
       <c r="L20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
         <v>10</v>
       </c>
-      <c r="M20" s="8">
-        <v>1</v>
-      </c>
       <c r="N20" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -1648,16 +1724,19 @@
         <v>124</v>
       </c>
       <c r="L21" s="10">
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
         <v>375</v>
       </c>
-      <c r="M21" s="8">
-        <v>1</v>
-      </c>
       <c r="N21" s="8">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -1689,16 +1768,19 @@
         <v>124</v>
       </c>
       <c r="L22" s="10">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10">
         <v>10000</v>
       </c>
-      <c r="M22" s="8">
-        <v>1</v>
-      </c>
       <c r="N22" s="8">
+        <v>1</v>
+      </c>
+      <c r="O22" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -1730,16 +1812,19 @@
         <v>124</v>
       </c>
       <c r="L23" s="10">
+        <v>1</v>
+      </c>
+      <c r="M23" s="10">
         <v>125000</v>
       </c>
-      <c r="M23" s="8">
-        <v>1</v>
-      </c>
       <c r="N23" s="8">
+        <v>1</v>
+      </c>
+      <c r="O23" s="8">
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -1771,16 +1856,19 @@
         <v>124</v>
       </c>
       <c r="L24" s="10">
+        <v>1</v>
+      </c>
+      <c r="M24" s="10">
         <v>7500000</v>
       </c>
-      <c r="M24" s="8">
-        <v>1</v>
-      </c>
       <c r="N24" s="8">
+        <v>1</v>
+      </c>
+      <c r="O24" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -1812,16 +1900,19 @@
         <v>124</v>
       </c>
       <c r="L25" s="10">
+        <v>1</v>
+      </c>
+      <c r="M25" s="10">
         <v>200000000</v>
       </c>
-      <c r="M25" s="8">
-        <v>1</v>
-      </c>
       <c r="N25" s="8">
+        <v>1</v>
+      </c>
+      <c r="O25" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>118</v>
       </c>
@@ -1855,14 +1946,17 @@
       <c r="L26" s="10">
         <v>1</v>
       </c>
-      <c r="M26" s="8">
-        <v>1</v>
+      <c r="M26" s="10">
+        <v>0</v>
       </c>
       <c r="N26" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -1896,14 +1990,17 @@
       <c r="L27" s="10">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M27" s="8">
-        <v>1</v>
+      <c r="M27" s="10">
+        <v>0</v>
       </c>
       <c r="N27" s="8">
+        <v>1</v>
+      </c>
+      <c r="O27" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -1937,14 +2034,17 @@
       <c r="L28" s="10">
         <v>1.000006</v>
       </c>
-      <c r="M28" s="8">
-        <v>1</v>
+      <c r="M28" s="10">
+        <v>0</v>
       </c>
       <c r="N28" s="8">
+        <v>1</v>
+      </c>
+      <c r="O28" s="8">
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -1978,14 +2078,17 @@
       <c r="L29" s="10">
         <v>1</v>
       </c>
-      <c r="M29" s="8">
-        <v>1</v>
+      <c r="M29" s="10">
+        <v>0</v>
       </c>
       <c r="N29" s="8">
+        <v>1</v>
+      </c>
+      <c r="O29" s="8">
         <v>200000</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -2019,14 +2122,17 @@
       <c r="L30" s="10">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M30" s="8">
-        <v>1</v>
+      <c r="M30" s="10">
+        <v>0</v>
       </c>
       <c r="N30" s="8">
+        <v>1</v>
+      </c>
+      <c r="O30" s="8">
         <v>1000000</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -2060,10 +2166,13 @@
       <c r="L31" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M31" s="8">
-        <v>1</v>
+      <c r="M31" s="10">
+        <v>0</v>
       </c>
       <c r="N31" s="8">
+        <v>1</v>
+      </c>
+      <c r="O31" s="8">
         <v>10000</v>
       </c>
     </row>
@@ -2083,7 +2192,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2262,7 @@
     <col min="5" max="6" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9" style="4"/>
     <col min="10" max="10" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2883,11 +2992,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -2999,156 +3108,225 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
       <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s">
         <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished connecting Buildings to excel
</commit_message>
<xml_diff>
--- a/Notes/Data.xlsx
+++ b/Notes/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="28800" windowHeight="12420" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Buildings" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
   <si>
     <t>US</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>unit018</t>
+  </si>
+  <si>
+    <t>isActive</t>
   </si>
 </sst>
 </file>
@@ -789,7 +792,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,63 +2187,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>126</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3110,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Military Data from Excel
</commit_message>
<xml_diff>
--- a/Notes/Data.xlsx
+++ b/Notes/Data.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="28800" windowHeight="12420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Buildings" sheetId="3" r:id="rId1"/>
     <sheet name="BuildingType" sheetId="5" r:id="rId2"/>
     <sheet name="Units" sheetId="2" r:id="rId3"/>
-    <sheet name="WorldCountries" sheetId="1" r:id="rId4"/>
-    <sheet name="CountryUnitArmyCode" sheetId="4" r:id="rId5"/>
+    <sheet name="UnitType" sheetId="6" r:id="rId4"/>
+    <sheet name="WorldCountries" sheetId="1" r:id="rId5"/>
+    <sheet name="CountryUnitArmyCode" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="146">
   <si>
     <t>US</t>
   </si>
@@ -75,9 +76,6 @@
     <t>siege</t>
   </si>
   <si>
-    <t>isUnlocked</t>
-  </si>
-  <si>
     <t>Militia</t>
   </si>
   <si>
@@ -189,9 +187,6 @@
     <t>MI</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -442,6 +437,36 @@
   </si>
   <si>
     <t>isActive</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Naval</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>unitTypeCode</t>
+  </si>
+  <si>
+    <t>unitTypeName</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>unlocked</t>
   </si>
 </sst>
 </file>
@@ -497,18 +522,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,1382 +824,1382 @@
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="8">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="8">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="10">
-        <v>1</v>
-      </c>
-      <c r="M2" s="10">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8">
-        <v>1</v>
-      </c>
-      <c r="O2" s="8">
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
+        <v>69</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
         <v>100</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>50000</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>50000</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <v>50000</v>
       </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="10">
+        <v>70</v>
+      </c>
+      <c r="L3" s="8">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M3" s="10">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>1</v>
-      </c>
-      <c r="O3" s="8">
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+        <v>69</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
         <v>2000</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>1000000</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>1000000</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>1000000</v>
       </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6">
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="10">
+        <v>70</v>
+      </c>
+      <c r="L4" s="8">
         <v>1.000006</v>
       </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>1</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
+        <v>69</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
         <v>100000</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>100000000</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>100000000</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>100000000</v>
       </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
         <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="10">
-        <v>0</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8">
+        <v>70</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
+        <v>69</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
         <v>200000</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>500000000</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>500000000</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <v>500000000</v>
       </c>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8">
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="10">
+        <v>70</v>
+      </c>
+      <c r="L6" s="8">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M6" s="10">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>1</v>
-      </c>
-      <c r="O6" s="8">
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
+        <v>69</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
         <v>1000000</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>10000000000</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>10000000000</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>10000000000</v>
       </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="10">
+        <v>70</v>
+      </c>
+      <c r="L7" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M7" s="10">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
-        <v>1</v>
-      </c>
-      <c r="O7" s="8">
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+      <c r="O7" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
+        <v>53</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
         <v>1000</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>1000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <v>1000</v>
       </c>
-      <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8">
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" s="10">
-        <v>1</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0</v>
-      </c>
-      <c r="N8" s="8">
-        <v>1</v>
-      </c>
-      <c r="O8" s="8">
+        <v>70</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
         <v>100</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>50000</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>50000</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <v>50000</v>
       </c>
-      <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
         <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" s="10">
+        <v>70</v>
+      </c>
+      <c r="L9" s="8">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M9" s="10">
-        <v>0</v>
-      </c>
-      <c r="N9" s="8">
-        <v>1</v>
-      </c>
-      <c r="O9" s="8">
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>1</v>
+      </c>
+      <c r="O9" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
+        <v>53</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
         <v>2000</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>1000000</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>1000000</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <v>1000000</v>
       </c>
-      <c r="I10" s="8">
-        <v>1</v>
-      </c>
-      <c r="J10" s="8">
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="10">
+        <v>70</v>
+      </c>
+      <c r="L10" s="8">
         <v>1.000006</v>
       </c>
-      <c r="M10" s="10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="8">
-        <v>1</v>
-      </c>
-      <c r="O10" s="8">
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
         <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
         <v>100000</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>100000000</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>100000000</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <v>100000000</v>
       </c>
-      <c r="I11" s="8">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" s="10">
-        <v>1</v>
-      </c>
-      <c r="M11" s="10">
-        <v>0</v>
-      </c>
-      <c r="N11" s="8">
-        <v>1</v>
-      </c>
-      <c r="O11" s="8">
+        <v>70</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>200000</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>500000000</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>500000000</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <v>500000000</v>
       </c>
-      <c r="I12" s="8">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8">
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
-      </c>
-      <c r="L12" s="10">
+        <v>70</v>
+      </c>
+      <c r="L12" s="8">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M12" s="10">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
-        <v>1</v>
-      </c>
-      <c r="O12" s="8">
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
         <v>1000000</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
         <v>1000000</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>10000000000</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <v>10000000000</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <v>10000000000</v>
       </c>
-      <c r="I13" s="8">
-        <v>1</v>
-      </c>
-      <c r="J13" s="8">
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
-      </c>
-      <c r="L13" s="10">
+        <v>70</v>
+      </c>
+      <c r="L13" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M13" s="10">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>1</v>
-      </c>
-      <c r="O13" s="8">
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="6">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="8">
-        <v>8</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1000</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1000</v>
-      </c>
-      <c r="H14" s="8">
-        <v>1000</v>
-      </c>
-      <c r="I14" s="8">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>111</v>
-      </c>
-      <c r="L14" s="10">
-        <v>1</v>
-      </c>
-      <c r="M14" s="10">
-        <v>1</v>
-      </c>
-      <c r="N14" s="8">
-        <v>1</v>
-      </c>
-      <c r="O14" s="8">
+      <c r="L14" s="8">
+        <v>1</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>200</v>
+      </c>
+      <c r="F15" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="6">
+        <v>100000</v>
+      </c>
+      <c r="H15" s="6">
+        <v>100000</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>200</v>
-      </c>
-      <c r="F15" s="8">
-        <v>100000</v>
-      </c>
-      <c r="G15" s="8">
-        <v>100000</v>
-      </c>
-      <c r="H15" s="8">
-        <v>100000</v>
-      </c>
-      <c r="I15" s="8">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
-        <v>2</v>
-      </c>
-      <c r="K15" t="s">
-        <v>111</v>
-      </c>
-      <c r="L15" s="10">
-        <v>1</v>
-      </c>
-      <c r="M15" s="10">
+      <c r="L15" s="8">
+        <v>1</v>
+      </c>
+      <c r="M15" s="8">
         <v>150</v>
       </c>
-      <c r="N15" s="8">
-        <v>1</v>
-      </c>
-      <c r="O15" s="8">
+      <c r="N15" s="6">
+        <v>1</v>
+      </c>
+      <c r="O15" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2000</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8">
         <v>2000</v>
       </c>
-      <c r="F16" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="I16" s="8">
-        <v>1</v>
-      </c>
-      <c r="J16" s="8">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
-        <v>111</v>
-      </c>
-      <c r="L16" s="10">
-        <v>1</v>
-      </c>
-      <c r="M16" s="10">
-        <v>2000</v>
-      </c>
-      <c r="N16" s="8">
-        <v>1</v>
-      </c>
-      <c r="O16" s="8">
+      <c r="N16" s="6">
+        <v>1</v>
+      </c>
+      <c r="O16" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="6">
+        <v>100000000</v>
+      </c>
+      <c r="G17" s="6">
+        <v>100000000</v>
+      </c>
+      <c r="H17" s="6">
+        <v>100000000</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
-        <v>100000</v>
-      </c>
-      <c r="F17" s="8">
-        <v>100000000</v>
-      </c>
-      <c r="G17" s="8">
-        <v>100000000</v>
-      </c>
-      <c r="H17" s="8">
-        <v>100000000</v>
-      </c>
-      <c r="I17" s="8">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8">
-        <v>4</v>
-      </c>
-      <c r="K17" t="s">
-        <v>111</v>
-      </c>
-      <c r="L17" s="10">
-        <v>1</v>
-      </c>
-      <c r="M17" s="10">
+      <c r="L17" s="8">
+        <v>1</v>
+      </c>
+      <c r="M17" s="8">
         <v>250000</v>
       </c>
-      <c r="N17" s="8">
-        <v>1</v>
-      </c>
-      <c r="O17" s="8">
+      <c r="N17" s="6">
+        <v>1</v>
+      </c>
+      <c r="O17" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
         <v>107</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>200000</v>
+      </c>
+      <c r="F18" s="6">
+        <v>500000000</v>
+      </c>
+      <c r="G18" s="6">
+        <v>500000000</v>
+      </c>
+      <c r="H18" s="6">
+        <v>500000000</v>
+      </c>
+      <c r="I18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6">
+        <v>5</v>
+      </c>
+      <c r="K18" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>200000</v>
-      </c>
-      <c r="F18" s="8">
-        <v>500000000</v>
-      </c>
-      <c r="G18" s="8">
-        <v>500000000</v>
-      </c>
-      <c r="H18" s="8">
-        <v>500000000</v>
-      </c>
-      <c r="I18" s="8">
-        <v>1</v>
-      </c>
-      <c r="J18" s="8">
-        <v>5</v>
-      </c>
-      <c r="K18" t="s">
-        <v>111</v>
-      </c>
-      <c r="L18" s="10">
-        <v>1</v>
-      </c>
-      <c r="M18" s="10">
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18" s="8">
         <v>1500000</v>
       </c>
-      <c r="N18" s="8">
-        <v>1</v>
-      </c>
-      <c r="O18" s="8">
+      <c r="N18" s="6">
+        <v>1</v>
+      </c>
+      <c r="O18" s="6">
         <v>50000</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="F19" s="6">
+        <v>10000000000</v>
+      </c>
+      <c r="G19" s="6">
+        <v>10000000000</v>
+      </c>
+      <c r="H19" s="6">
+        <v>10000000000</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="F19" s="8">
-        <v>10000000000</v>
-      </c>
-      <c r="G19" s="8">
-        <v>10000000000</v>
-      </c>
-      <c r="H19" s="8">
-        <v>10000000000</v>
-      </c>
-      <c r="I19" s="8">
-        <v>1</v>
-      </c>
-      <c r="J19" s="8">
-        <v>6</v>
-      </c>
-      <c r="K19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L19" s="10">
-        <v>1</v>
-      </c>
-      <c r="M19" s="10">
+      <c r="L19" s="8">
+        <v>1</v>
+      </c>
+      <c r="M19" s="8">
         <v>40000000</v>
       </c>
-      <c r="N19" s="8">
-        <v>1</v>
-      </c>
-      <c r="O19" s="8">
+      <c r="N19" s="6">
+        <v>1</v>
+      </c>
+      <c r="O19" s="6">
         <v>100000</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="8">
+        <v>52</v>
+      </c>
+      <c r="D20" s="6">
         <v>5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>2</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>2000</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="6">
         <v>2000</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="6">
         <v>2000</v>
       </c>
-      <c r="I20" s="8">
-        <v>1</v>
-      </c>
-      <c r="J20" s="8">
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>124</v>
-      </c>
-      <c r="L20" s="10">
-        <v>1</v>
-      </c>
-      <c r="M20" s="10">
+        <v>122</v>
+      </c>
+      <c r="L20" s="8">
+        <v>1</v>
+      </c>
+      <c r="M20" s="8">
         <v>10</v>
       </c>
-      <c r="N20" s="8">
-        <v>1</v>
-      </c>
-      <c r="O20" s="8">
+      <c r="N20" s="6">
+        <v>1</v>
+      </c>
+      <c r="O20" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
+        <v>52</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
         <v>100</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="6">
         <v>50000</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="6">
         <v>50000</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="6">
         <v>50000</v>
       </c>
-      <c r="I21" s="8">
-        <v>1</v>
-      </c>
-      <c r="J21" s="8">
+      <c r="I21" s="6">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6">
         <v>2</v>
       </c>
       <c r="K21" t="s">
-        <v>124</v>
-      </c>
-      <c r="L21" s="10">
-        <v>1</v>
-      </c>
-      <c r="M21" s="10">
+        <v>122</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+      <c r="M21" s="8">
         <v>375</v>
       </c>
-      <c r="N21" s="8">
-        <v>1</v>
-      </c>
-      <c r="O21" s="8">
+      <c r="N21" s="6">
+        <v>1</v>
+      </c>
+      <c r="O21" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
+        <v>52</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
         <v>2000</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="6">
         <v>1000000</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="6">
         <v>1000000</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="6">
         <v>1000000</v>
       </c>
-      <c r="I22" s="8">
-        <v>1</v>
-      </c>
-      <c r="J22" s="8">
+      <c r="I22" s="6">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6">
         <v>3</v>
       </c>
       <c r="K22" t="s">
-        <v>124</v>
-      </c>
-      <c r="L22" s="10">
-        <v>1</v>
-      </c>
-      <c r="M22" s="10">
+        <v>122</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8">
         <v>10000</v>
       </c>
-      <c r="N22" s="8">
-        <v>1</v>
-      </c>
-      <c r="O22" s="8">
+      <c r="N22" s="6">
+        <v>1</v>
+      </c>
+      <c r="O22" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
+        <v>52</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
         <v>10000</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>10000000</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>10000000</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>10000000</v>
       </c>
-      <c r="I23" s="8">
-        <v>1</v>
-      </c>
-      <c r="J23" s="8">
+      <c r="I23" s="6">
+        <v>1</v>
+      </c>
+      <c r="J23" s="6">
         <v>4</v>
       </c>
       <c r="K23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L23" s="10">
-        <v>1</v>
-      </c>
-      <c r="M23" s="10">
+        <v>122</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+      <c r="M23" s="8">
         <v>125000</v>
       </c>
-      <c r="N23" s="8">
-        <v>1</v>
-      </c>
-      <c r="O23" s="8">
+      <c r="N23" s="6">
+        <v>1</v>
+      </c>
+      <c r="O23" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8">
+        <v>52</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
         <v>200000</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="6">
         <v>500000000</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="6">
         <v>500000000</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="6">
         <v>500000000</v>
       </c>
-      <c r="I24" s="8">
-        <v>1</v>
-      </c>
-      <c r="J24" s="8">
+      <c r="I24" s="6">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6">
         <v>5</v>
       </c>
       <c r="K24" t="s">
-        <v>124</v>
-      </c>
-      <c r="L24" s="10">
-        <v>1</v>
-      </c>
-      <c r="M24" s="10">
+        <v>122</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+      <c r="M24" s="8">
         <v>7500000</v>
       </c>
-      <c r="N24" s="8">
-        <v>1</v>
-      </c>
-      <c r="O24" s="8">
+      <c r="N24" s="6">
+        <v>1</v>
+      </c>
+      <c r="O24" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="8">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8">
+        <v>52</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
         <v>1000000</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="6">
         <v>10000000000</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="6">
         <v>10000000000</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="6">
         <v>10000000000</v>
       </c>
-      <c r="I25" s="8">
-        <v>1</v>
-      </c>
-      <c r="J25" s="8">
+      <c r="I25" s="6">
+        <v>1</v>
+      </c>
+      <c r="J25" s="6">
         <v>6</v>
       </c>
       <c r="K25" t="s">
-        <v>124</v>
-      </c>
-      <c r="L25" s="10">
-        <v>1</v>
-      </c>
-      <c r="M25" s="10">
+        <v>122</v>
+      </c>
+      <c r="L25" s="8">
+        <v>1</v>
+      </c>
+      <c r="M25" s="8">
         <v>200000000</v>
       </c>
-      <c r="N25" s="8">
-        <v>1</v>
-      </c>
-      <c r="O25" s="8">
+      <c r="N25" s="6">
+        <v>1</v>
+      </c>
+      <c r="O25" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
+        <v>108</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
         <v>1000</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="6">
         <v>1000</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="6">
         <v>1000</v>
       </c>
-      <c r="I26" s="8">
-        <v>1</v>
-      </c>
-      <c r="J26" s="8">
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" s="10">
-        <v>1</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0</v>
-      </c>
-      <c r="N26" s="8">
-        <v>1</v>
-      </c>
-      <c r="O26" s="8">
+        <v>70</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1</v>
+      </c>
+      <c r="M26" s="8">
+        <v>0</v>
+      </c>
+      <c r="N26" s="6">
+        <v>1</v>
+      </c>
+      <c r="O26" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="8">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8">
+        <v>108</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
         <v>100</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <v>50000</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="6">
         <v>50000</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="6">
         <v>50000</v>
       </c>
-      <c r="I27" s="8">
-        <v>1</v>
-      </c>
-      <c r="J27" s="8">
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6">
         <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="10">
+        <v>70</v>
+      </c>
+      <c r="L27" s="8">
         <v>1.0000001000000001</v>
       </c>
-      <c r="M27" s="10">
-        <v>0</v>
-      </c>
-      <c r="N27" s="8">
-        <v>1</v>
-      </c>
-      <c r="O27" s="8">
+      <c r="M27" s="8">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6">
+        <v>1</v>
+      </c>
+      <c r="O27" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="8">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
+        <v>108</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
         <v>2000</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <v>1000000</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="6">
         <v>1000000</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="6">
         <v>1000000</v>
       </c>
-      <c r="I28" s="8">
-        <v>1</v>
-      </c>
-      <c r="J28" s="8">
+      <c r="I28" s="6">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6">
         <v>3</v>
       </c>
       <c r="K28" t="s">
-        <v>72</v>
-      </c>
-      <c r="L28" s="10">
+        <v>70</v>
+      </c>
+      <c r="L28" s="8">
         <v>1.000006</v>
       </c>
-      <c r="M28" s="10">
-        <v>0</v>
-      </c>
-      <c r="N28" s="8">
-        <v>1</v>
-      </c>
-      <c r="O28" s="8">
+      <c r="M28" s="8">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
+        <v>1</v>
+      </c>
+      <c r="O28" s="6">
         <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="8">
-        <v>0</v>
-      </c>
-      <c r="E29" s="8">
+        <v>108</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
         <v>100000</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>100000000</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="6">
         <v>100000000</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="6">
         <v>100000000</v>
       </c>
-      <c r="I29" s="8">
-        <v>1</v>
-      </c>
-      <c r="J29" s="8">
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
         <v>4</v>
       </c>
       <c r="K29" t="s">
-        <v>72</v>
-      </c>
-      <c r="L29" s="10">
-        <v>1</v>
-      </c>
-      <c r="M29" s="10">
-        <v>0</v>
-      </c>
-      <c r="N29" s="8">
-        <v>1</v>
-      </c>
-      <c r="O29" s="8">
+        <v>70</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0</v>
+      </c>
+      <c r="N29" s="6">
+        <v>1</v>
+      </c>
+      <c r="O29" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="8">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8">
+        <v>108</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6">
         <v>200000</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="6">
         <v>500000000</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="6">
         <v>500000000</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="6">
         <v>500000000</v>
       </c>
-      <c r="I30" s="8">
-        <v>1</v>
-      </c>
-      <c r="J30" s="8">
+      <c r="I30" s="6">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6">
         <v>5</v>
       </c>
       <c r="K30" t="s">
-        <v>72</v>
-      </c>
-      <c r="L30" s="10">
+        <v>70</v>
+      </c>
+      <c r="L30" s="8">
         <v>1.0035000000000001</v>
       </c>
-      <c r="M30" s="10">
-        <v>0</v>
-      </c>
-      <c r="N30" s="8">
-        <v>1</v>
-      </c>
-      <c r="O30" s="8">
+      <c r="M30" s="8">
+        <v>0</v>
+      </c>
+      <c r="N30" s="6">
+        <v>1</v>
+      </c>
+      <c r="O30" s="6">
         <v>1000000</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="8">
-        <v>0</v>
-      </c>
-      <c r="E31" s="8">
+        <v>108</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
         <v>1000000</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <v>10000000000</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="6">
         <v>10000000000</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="6">
         <v>10000000000</v>
       </c>
-      <c r="I31" s="8">
-        <v>1</v>
-      </c>
-      <c r="J31" s="8">
+      <c r="I31" s="6">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6">
         <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>72</v>
-      </c>
-      <c r="L31" s="10">
+        <v>70</v>
+      </c>
+      <c r="L31" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M31" s="10">
-        <v>0</v>
-      </c>
-      <c r="N31" s="8">
-        <v>1</v>
-      </c>
-      <c r="O31" s="8">
+      <c r="M31" s="8">
+        <v>0</v>
+      </c>
+      <c r="N31" s="6">
+        <v>1</v>
+      </c>
+      <c r="O31" s="6">
         <v>10000</v>
       </c>
     </row>
@@ -2189,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,22 +2224,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>137</v>
+      <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2223,10 +2247,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2234,10 +2258,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2245,10 +2269,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2256,10 +2280,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2274,17 +2298,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9" style="4"/>
-    <col min="10" max="10" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="6"/>
+    <col min="9" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2297,69 +2324,69 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4">
+        <v>136</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6">
         <v>0</v>
       </c>
       <c r="M2" t="b">
@@ -2368,37 +2395,37 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4">
+        <v>136</v>
+      </c>
+      <c r="E3" s="6">
         <v>19</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>19</v>
       </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
         <v>2</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="6">
         <v>5</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="6">
         <v>5</v>
       </c>
-      <c r="L3" s="4">
-        <v>0.1</v>
+      <c r="L3" s="6">
+        <v>1</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -2406,36 +2433,36 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="4">
-        <v>10000</v>
-      </c>
-      <c r="F4" s="4">
-        <v>10000</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>5</v>
-      </c>
-      <c r="I4" s="4">
-        <v>20</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="J4" s="6">
         <v>10</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="6">
         <v>1000</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="6">
         <v>5000</v>
       </c>
       <c r="M4" t="b">
@@ -2444,36 +2471,36 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4">
+        <v>136</v>
+      </c>
+      <c r="E5" s="6">
         <v>100000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <v>100000</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
         <v>20</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="6">
         <v>100</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="6">
         <v>30000</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="6">
         <v>1000</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="6">
         <v>1000</v>
       </c>
       <c r="M5" t="b">
@@ -2482,36 +2509,36 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4">
+        <v>136</v>
+      </c>
+      <c r="E6" s="6">
         <v>10000000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="6">
         <v>10000000</v>
       </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
         <v>50</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="6">
         <v>750</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="6">
         <v>1000000</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="6">
         <v>1000000</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="6">
         <v>1000000</v>
       </c>
       <c r="M6" t="b">
@@ -2520,36 +2547,36 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4">
+        <v>136</v>
+      </c>
+      <c r="E7" s="6">
         <v>100000000</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="6">
         <v>100000000</v>
       </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
         <v>100</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>1000</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="6">
         <v>10000000</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="6">
         <v>1000000</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="6">
         <v>100000</v>
       </c>
       <c r="M7" t="b">
@@ -2558,36 +2585,36 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>10</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="6">
         <v>10</v>
       </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
         <v>3</v>
       </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
         <v>10</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="6">
         <v>10</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="6">
         <v>0</v>
       </c>
       <c r="M8" t="b">
@@ -2596,36 +2623,36 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6">
         <v>10000</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="6">
         <v>10000</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
         <v>20</v>
       </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
         <v>8000</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="6">
         <v>1000</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="6">
         <v>2000</v>
       </c>
       <c r="M9" t="b">
@@ -2634,36 +2661,36 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="4">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6">
         <v>100000</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="6">
         <v>100000</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>100</v>
       </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
         <v>10000</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="6">
         <v>100000</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="6">
         <v>1000</v>
       </c>
       <c r="M10" t="b">
@@ -2672,36 +2699,36 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="4">
+        <v>28</v>
+      </c>
+      <c r="E11" s="6">
         <v>10000000</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="6">
         <v>10000000</v>
       </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
         <v>1000</v>
       </c>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
         <v>1000000</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="6">
         <v>1000000</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="6">
         <v>3000000</v>
       </c>
       <c r="M11" t="b">
@@ -2710,36 +2737,36 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
       <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6">
         <v>100000000</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="6">
         <v>100000000</v>
       </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
         <v>2000</v>
       </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
         <v>100000000</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="6">
         <v>80000000</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="6">
         <v>50000000</v>
       </c>
       <c r="M12" t="b">
@@ -2748,36 +2775,36 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
       <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="4">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6">
         <v>10000</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="6">
         <v>10000</v>
       </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
         <v>5</v>
       </c>
-      <c r="I13" s="4">
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
         <v>10000</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="6">
         <v>10000</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="6">
         <v>1</v>
       </c>
       <c r="M13" t="b">
@@ -2786,36 +2813,36 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
       <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="4">
+        <v>25</v>
+      </c>
+      <c r="E14" s="6">
         <v>100000</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="6">
         <v>100000</v>
       </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
         <v>2</v>
       </c>
-      <c r="I14" s="4">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
         <v>100000</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="6">
         <v>10000</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="6">
         <v>1000</v>
       </c>
       <c r="M14" t="b">
@@ -2824,36 +2851,36 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="4">
+        <v>25</v>
+      </c>
+      <c r="E15" s="6">
         <v>1000000</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="6">
         <v>1000000</v>
       </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
         <v>20</v>
       </c>
-      <c r="I15" s="4">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
         <v>100000</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="6">
         <v>300000</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="6">
         <v>300000</v>
       </c>
       <c r="M15" t="b">
@@ -2862,36 +2889,36 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="4">
+        <v>25</v>
+      </c>
+      <c r="E16" s="6">
         <v>10000000</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="6">
         <v>10000000</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
         <v>50</v>
       </c>
-      <c r="I16" s="4">
-        <v>1</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
         <v>500000</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="6">
         <v>2000000</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="6">
         <v>2000000</v>
       </c>
       <c r="M16" t="b">
@@ -2900,36 +2927,36 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="4">
+        <v>25</v>
+      </c>
+      <c r="E17" s="6">
         <v>100000000</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="6">
         <v>100000000</v>
       </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
         <v>5</v>
       </c>
-      <c r="I17" s="4">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6">
         <v>10000000</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="6">
         <v>100000</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="6">
         <v>20000000</v>
       </c>
       <c r="M17" t="b">
@@ -2938,36 +2965,36 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="4">
+        <v>25</v>
+      </c>
+      <c r="E18" s="6">
         <v>1000000000</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="6">
         <v>1000000000</v>
       </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
         <v>10000</v>
       </c>
-      <c r="I18" s="4">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="I18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6">
         <v>10000000</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="6">
         <v>100000000</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="6">
         <v>10000000</v>
       </c>
       <c r="M18" t="b">
@@ -2976,26 +3003,116 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="E19" s="6">
+        <v>50000</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <v>5000</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K19" s="6">
+        <v>100</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="E20" s="6">
+        <v>100000</v>
+      </c>
+      <c r="F20" s="6">
+        <v>100</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1</v>
+      </c>
+      <c r="I20" s="6">
+        <v>100000</v>
+      </c>
+      <c r="J20" s="6">
+        <v>5</v>
+      </c>
+      <c r="K20" s="6">
+        <v>10</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="E21" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F21" s="6">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6">
+        <v>200000</v>
+      </c>
+      <c r="J21" s="6">
+        <v>500</v>
+      </c>
+      <c r="K21" s="6">
+        <v>500</v>
+      </c>
+      <c r="L21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3005,6 +3122,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -3018,75 +3207,75 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="M1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -3101,9 +3290,9 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="6">
+        <v>28</v>
+      </c>
+      <c r="F2" s="4">
         <v>100000000</v>
       </c>
     </row>
@@ -3119,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -3144,211 +3333,211 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>